<commit_message>
Fanlara kadar(fanlar dahil) kurulum ayarları kısmı tamamlandı.
</commit_message>
<xml_diff>
--- a/database_haritası.xlsx
+++ b/database_haritası.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kontrol A\flutteruygulamalar\prokos_beta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C96E654-5E44-4E5E-A9DE-969CA84D36A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5634CD9A-2D88-42B5-A00C-7B853D8B59D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{295E6919-D699-430A-8921-C9E488B05D0D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{295E6919-D699-430A-8921-C9E488B05D0D}"/>
   </bookViews>
   <sheets>
     <sheet name="EkranDatabase" sheetId="1" r:id="rId1"/>
     <sheet name="ServerDBKurulum" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
   <si>
     <t>ID NO</t>
   </si>
@@ -153,18 +154,6 @@
     <t>Dış Nem</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>FanHarita Şekil1</t>
-  </si>
-  <si>
-    <t>FanHarita Şekil 120</t>
-  </si>
-  <si>
-    <t>fanHaritaOnay</t>
-  </si>
-  <si>
     <t>Temel Ayarlar Durum(ok veya null)</t>
   </si>
   <si>
@@ -244,6 +233,39 @@
   </si>
   <si>
     <t>C(m)</t>
+  </si>
+  <si>
+    <t>Debi ve Nem Durum(ok veya null)</t>
+  </si>
+  <si>
+    <t>Tfan Debi</t>
+  </si>
+  <si>
+    <t>Bfan Debi</t>
+  </si>
+  <si>
+    <t>Fan Harita Durum(ok veya null)</t>
+  </si>
+  <si>
+    <t>Fan Harita Konumları</t>
+  </si>
+  <si>
+    <t>fan Harita Onay</t>
+  </si>
+  <si>
+    <t>çıkışNo'lar</t>
+  </si>
+  <si>
+    <t>fanHarita'lar</t>
+  </si>
+  <si>
+    <t>Fan ve Çıkış No Onay</t>
+  </si>
+  <si>
+    <t>fanNo'lar</t>
+  </si>
+  <si>
+    <t>Fan No ve Çıkış No Durum(ok veya null)</t>
   </si>
 </sst>
 </file>
@@ -633,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45BE288-E241-4B33-BEDB-2CBD76C7D48D}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -926,122 +948,43 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="2">
-        <v>1001</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0</v>
-      </c>
-      <c r="F20" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="2">
-        <v>1120</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0</v>
-      </c>
-      <c r="E25" s="2">
-        <v>0</v>
-      </c>
-      <c r="F25" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="2">
-        <v>1121</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0</v>
-      </c>
-      <c r="F26" s="2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1054,17 +997,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B1A72B-8FB3-40DC-96DB-18BF28E0347C}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="33.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="21" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1096,7 +1039,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
@@ -1116,16 +1059,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1136,7 +1079,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -1156,16 +1099,16 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1176,7 +1119,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
@@ -1196,16 +1139,16 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1216,10 +1159,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
@@ -1236,7 +1179,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>21</v>
@@ -1256,10 +1199,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>
@@ -1276,7 +1219,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
@@ -1316,7 +1259,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
@@ -1356,7 +1299,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
@@ -1396,16 +1339,96 @@
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2">
+        <v>17</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2">
+        <v>18</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="E19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>70</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Klepelere kadar(klepeler dahil) kurulum ayarları kısmı tamamlandı.
</commit_message>
<xml_diff>
--- a/database_haritası.xlsx
+++ b/database_haritası.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kontrol A\flutteruygulamalar\prokos_beta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5634CD9A-2D88-42B5-A00C-7B853D8B59D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052534CB-5CC4-43C1-9AD3-642584DC604A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{295E6919-D699-430A-8921-C9E488B05D0D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{295E6919-D699-430A-8921-C9E488B05D0D}"/>
   </bookViews>
   <sheets>
     <sheet name="EkranDatabase" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="84">
   <si>
     <t>ID NO</t>
   </si>
@@ -266,6 +266,24 @@
   </si>
   <si>
     <t>Fan No ve Çıkış No Durum(ok veya null)</t>
+  </si>
+  <si>
+    <t>Klepe Harita Onay</t>
+  </si>
+  <si>
+    <t>klepeHaritalar</t>
+  </si>
+  <si>
+    <t>Klepe ve Çıkış No Onay</t>
+  </si>
+  <si>
+    <t>klepeNo'lar</t>
+  </si>
+  <si>
+    <t>cikisNo'lar</t>
+  </si>
+  <si>
+    <t>Klepe No ve Çıkış No Durum(ok veya null)</t>
   </si>
 </sst>
 </file>
@@ -655,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45BE288-E241-4B33-BEDB-2CBD76C7D48D}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,6 +1006,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2">
+        <v>17</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -997,17 +1055,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B1A72B-8FB3-40DC-96DB-18BF28E0347C}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" style="2" customWidth="1"/>
     <col min="4" max="6" width="21" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1431,6 +1489,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2">
+        <v>21</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ped Pompalarının kurulum ayarları kısmı tamamlandı.
</commit_message>
<xml_diff>
--- a/database_haritası.xlsx
+++ b/database_haritası.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kontrol A\flutteruygulamalar\prokos_beta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052534CB-5CC4-43C1-9AD3-642584DC604A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2594E4D3-5D02-4165-B5E0-F128A338ABDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{295E6919-D699-430A-8921-C9E488B05D0D}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="ServerDBKurulum" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="95">
   <si>
     <t>ID NO</t>
   </si>
@@ -284,6 +283,39 @@
   </si>
   <si>
     <t>Klepe No ve Çıkış No Durum(ok veya null)</t>
+  </si>
+  <si>
+    <t>Klepe Harita Durum(ok veya null)</t>
+  </si>
+  <si>
+    <t>Ped Harita Onay</t>
+  </si>
+  <si>
+    <t>Ped ve Çıkış No Onay</t>
+  </si>
+  <si>
+    <t>cikisNoAc'lar</t>
+  </si>
+  <si>
+    <t>cikisNoKapa'lar</t>
+  </si>
+  <si>
+    <t>çıkışNoAc'lar</t>
+  </si>
+  <si>
+    <t>çıkışNoKapa'lar</t>
+  </si>
+  <si>
+    <t>Ped Harita Durum(ok veya null)</t>
+  </si>
+  <si>
+    <t>Ped No ve Çıkış No Durum(ok veya null)</t>
+  </si>
+  <si>
+    <t>Klepe Harita Konumları</t>
+  </si>
+  <si>
+    <t>Ped Harita Konumları</t>
   </si>
 </sst>
 </file>
@@ -673,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45BE288-E241-4B33-BEDB-2CBD76C7D48D}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1040,9 +1072,49 @@
         <v>81</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2">
+        <v>18</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F20" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1055,10 +1127,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B1A72B-8FB3-40DC-96DB-18BF28E0347C}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1497,15 +1569,75 @@
         <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2">
+        <v>22</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2">
+        <v>24</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F25" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>